<commit_message>
[UPD] Added proper bootstrap and rearrange few parts
</commit_message>
<xml_diff>
--- a/exams/risultati_scritto.xlsx
+++ b/exams/risultati_scritto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\shared\finance_course\exams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34197AD1-D3C4-4070-8B2C-F23EF000F248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7CF218-5395-4698-B353-D411C6ABC388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11535" yWindow="-15045" windowWidth="27420" windowHeight="15045" activeTab="1" xr2:uid="{6CFE4764-E1FB-4DB6-AB83-5FACA4F3BFDE}"/>
+    <workbookView xWindow="-13260" yWindow="-14505" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{6CFE4764-E1FB-4DB6-AB83-5FACA4F3BFDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Question</t>
   </si>
@@ -61,16 +61,28 @@
     <t>Gianmarco Ottaviano</t>
   </si>
   <si>
-    <t>GIONA BIANCHI</t>
-  </si>
-  <si>
-    <t>ERICA ROMANO</t>
-  </si>
-  <si>
-    <t>FEDERICO SPINETTI</t>
-  </si>
-  <si>
     <t>Voti per esercizio da 0 a 6</t>
+  </si>
+  <si>
+    <t>Aryo Omrani</t>
+  </si>
+  <si>
+    <t>Yehya Ghaddar</t>
+  </si>
+  <si>
+    <t>Hamida Benhamed</t>
+  </si>
+  <si>
+    <t>Asalkhon Otakhonova</t>
+  </si>
+  <si>
+    <t>Rotislav Plotnikov</t>
+  </si>
+  <si>
+    <t>Mammadli Tofig</t>
+  </si>
+  <si>
+    <t>Questa studentessa non ha richiesto il progetto..</t>
   </si>
 </sst>
 </file>
@@ -129,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -164,6 +176,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -893,10 +911,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD9E31F-A6AA-4051-BC57-551296F8774A}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,9 +922,9 @@
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -917,17 +935,23 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -948,7 +972,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -971,7 +995,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -989,26 +1013,32 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
       </c>
       <c r="C5" s="10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1">
         <v>6</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="F5" s="1">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1">
+        <v>6</v>
+      </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1019,92 +1049,100 @@
         <v>5</v>
       </c>
       <c r="C6" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>6</v>
+      </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7" s="5">
         <v>6</v>
       </c>
       <c r="C7" s="11">
-        <v>3</v>
-      </c>
-      <c r="D7" s="6">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
       </c>
       <c r="E7" s="6">
-        <v>6</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>4</v>
+      </c>
+      <c r="G7" s="6">
+        <v>4</v>
+      </c>
+      <c r="H7" s="6">
+        <v>2</v>
+      </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8" s="5">
         <v>7</v>
       </c>
       <c r="C8" s="11">
-        <v>6</v>
-      </c>
-      <c r="D8" s="6">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
       </c>
       <c r="E8" s="6">
-        <v>6</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>5</v>
+      </c>
+      <c r="G8" s="6">
+        <v>6</v>
+      </c>
+      <c r="H8" s="6">
+        <v>5</v>
+      </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>4</v>
-      </c>
-      <c r="B9" s="7">
-        <v>8</v>
-      </c>
-      <c r="C9" s="12">
-        <v>6</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8">
-        <v>6</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="1">
+      <c r="I9" s="1" t="e">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1114,27 +1152,27 @@
       </c>
       <c r="C10" s="1">
         <f>SUMPRODUCT(C2:C9,$A2:$A9)/5</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" ref="D10:H10" si="1">SUMPRODUCT(D2:D9,$A2:$A9)/5</f>
-        <v>4</v>
+        <v>9.6</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>5.2</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.2</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.8</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1143,27 +1181,27 @@
       </c>
       <c r="C11" s="1">
         <f>+$B$11*C10+(1-$B$11)*C12</f>
-        <v>19.5</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <f>+$B$11*D10+(1-$B$11)*D12</f>
-        <v>10.5</v>
+        <v>14.7</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:H11" si="2">+$B$11*E10+(1-$B$11)*E12</f>
-        <v>21</v>
+        <v>11.4</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>7.5</v>
+        <v>16.649999999999999</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>7.5</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>7.5</v>
+        <v>15.45</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1184,6 +1222,11 @@
       </c>
       <c r="H12" s="1">
         <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="F14" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>